<commit_message>
Manual Coding Phase Defects detection and correction
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laptop\e\VVSS\CamiVVSS_ro2024-2025\Labs\Lab01\CheckListsAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geani\IdeaProjects\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C988F33-E974-4516-BC95-27D0B68ECC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1014614-33DF-4626-9AC8-3B2C176AE29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20436" yWindow="1164" windowWidth="21600" windowHeight="11772" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -135,19 +135,253 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>Chelaru Laurentiu</t>
+  </si>
+  <si>
+    <t>232/1</t>
+  </si>
+  <si>
+    <t>Ciubotariu Veronica</t>
+  </si>
+  <si>
+    <t>232/2</t>
+  </si>
+  <si>
+    <t>Ciulavu Dan Flaviu</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>OrdersGUI.java/line 22</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In loc sa pasam de fiecare data acelasi service functiei </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>displayOrdersForm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> am putea sa ne folosim de membrul privat al clasei si sa pasam o singura data service-ul. Putem introduce o functie </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">setService </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">si sa stergem parametrul functiei </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>displayOrdersForm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>Folosim rezultatul unui Optional fara sa verificam daca exista unul. Cazul de exceptie in care nu avem niciun rezultat trebuie tratat.</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>PizzaService.java/line 32</t>
+  </si>
+  <si>
+    <t>Ar trebui sa folosim nume de variabile mai sugestive. Propun urmtoarele inlocuiri: l -&gt; payments, p -&gt; payment</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java/line 150; PaymentAlert/line 46, 49</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>MenuRepository.java/line 48</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Meniul se citeste din fisier de fiecare data cand acesta este cerut din orice alta parte a aplicatie (apeland functia </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>getMenu</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">), desi acesta nu se modifica. Daca avem multe produse in meniu, acest fapt poate duce la probleme de performanta. Meniul ar trebui citit si incarcat la instantierea </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MenuRepository</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>KitchenGUIController/line 44</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cazul in care nu avem nicio comanda selectata nu este tratat corespunzator in actiunile butonaelor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cook </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ready</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Vom verifica daca avem o comanda selectata si in caz contrar vom notifica utilizatorul ca trebuie sa selecteze o comanda.</t>
+    </r>
+  </si>
+  <si>
+    <t>0.5h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,79 +560,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,36 +950,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -750,57 +988,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -814,7 +1052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -822,7 +1060,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -831,7 +1069,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -840,7 +1078,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -849,7 +1087,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -858,7 +1096,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -867,7 +1105,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -876,7 +1114,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -885,7 +1123,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -894,7 +1132,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -903,7 +1141,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -912,7 +1150,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -921,7 +1159,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -930,7 +1168,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -939,7 +1177,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -948,7 +1186,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -957,7 +1195,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -989,35 +1227,35 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1026,57 +1264,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1098,7 +1336,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1107,7 +1345,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1116,7 +1354,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1125,7 +1363,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1134,7 +1372,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1143,7 +1381,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1152,7 +1390,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1161,7 +1399,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1170,7 +1408,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1179,7 +1417,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1188,7 +1426,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1197,7 +1435,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1206,7 +1444,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1215,7 +1453,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1224,7 +1462,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1233,7 +1471,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1242,7 +1480,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1270,40 +1508,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1312,57 +1550,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="37">
+        <v>45872</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1376,51 +1630,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1429,7 +1713,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1438,7 +1722,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1447,7 +1731,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1456,7 +1740,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1465,7 +1749,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1474,7 +1758,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1483,7 +1767,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1492,7 +1776,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1501,7 +1785,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1510,7 +1794,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1519,7 +1803,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1528,7 +1812,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1537,7 +1821,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1546,7 +1830,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1555,7 +1839,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1564,12 +1848,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1592,41 +1878,41 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="5" max="5" width="23.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1635,47 +1921,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1701,7 +1987,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1711,7 +1997,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1721,7 +2007,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1731,7 +2017,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1741,7 +2027,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1751,7 +2037,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1761,7 +2047,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1771,7 +2057,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1781,7 +2067,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1791,7 +2077,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1801,7 +2087,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1811,7 +2097,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1821,7 +2107,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1831,7 +2117,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1841,7 +2127,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1851,7 +2137,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1861,7 +2147,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1871,7 +2157,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1881,7 +2167,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1891,7 +2177,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1901,16 +2187,16 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="33" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F35" s="35"/>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Coding Phase Defects detection and correction with SonarQube
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geani\IdeaProjects\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1014614-33DF-4626-9AC8-3B2C176AE29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ADB713-8377-4242-9696-833753D9952A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20436" yWindow="1164" windowWidth="21600" windowHeight="11772" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19092" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -363,12 +363,121 @@
   <si>
     <t>0.5h</t>
   </si>
+  <si>
+    <t>SonarQube</t>
+  </si>
+  <si>
+    <t>PaymentType.java/4</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cash, Card</t>
+  </si>
+  <si>
+    <t>Implementarea este strans legata de denumirea mambrilor acestui enum, iar schimbarea aceasta ar presupune tratarea sa in mai multe locuri, inclusiv la citirea platilor.</t>
+  </si>
+  <si>
+    <t>MenuRepository.java/24</t>
+  </si>
+  <si>
+    <t>Resources should be closed</t>
+  </si>
+  <si>
+    <t>try {
+            br = new BufferedReader(new FileReader(file));</t>
+  </si>
+  <si>
+    <t>try(FileReader fr = new FileReader(file); BufferedReader br = new BufferedReader(fr)) {</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>MenuRepository.java/19</t>
+  </si>
+  <si>
+    <t>//ClassLoader classLoader = MenuRepository.class.getClassLoader();</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Raw types should not be used</t>
+  </si>
+  <si>
+    <t>MenuRepository.java/20</t>
+  </si>
+  <si>
+    <t>this.listMenu= new ArrayList();</t>
+  </si>
+  <si>
+    <t>this.listMenu= new ArrayList&lt;&gt;();</t>
+  </si>
+  <si>
+    <t>Catches should be combined</t>
+  </si>
+  <si>
+    <t>MenuRepository.java/29</t>
+  </si>
+  <si>
+    <t>catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>PizzaService.java/33</t>
+  </si>
+  <si>
+    <t>"Collection.isEmpty()" should be used to test for emptiness</t>
+  </si>
+  <si>
+    <t>if ((payments==null) ||(payments.size()==0)) return total;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if ((payments==null) ||(payments.isEmpty())) return total;</t>
+  </si>
+  <si>
+    <t>OrdersGUI.java/31</t>
+  </si>
+  <si>
+    <t>//vBoxOrders = FXMLLoader.load(getClass().getResource("/fxml/OrdersGUIFXML.fxml"));</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Anonymous inner classes containing only one method should become lambdas</t>
+  </si>
+  <si>
+    <t>OrdersGUI.java/43</t>
+  </si>
+  <si>
+    <t>stage.setOnCloseRequest(new EventHandler&lt;WindowEvent&gt;() {
+      @Override
+     public void handle(WindowEvent event) {
+         // consume event
+         event.consume();
+            }
+        });</t>
+  </si>
+  <si>
+    <t>stage.setOnCloseRequest(Event::consume);</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +568,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF7A7E85"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -560,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -591,6 +706,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -618,6 +734,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -633,9 +752,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,7 +1068,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -962,24 +1080,24 @@
     <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -988,57 +1106,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1060,7 +1178,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1069,7 +1187,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1078,7 +1196,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1087,7 +1205,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1096,7 +1214,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1105,7 +1223,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1114,7 +1232,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1123,7 +1241,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1132,7 +1250,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1141,7 +1259,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1150,7 +1268,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1159,7 +1277,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1168,7 +1286,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1177,7 +1295,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1186,7 +1304,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1195,7 +1313,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1227,7 +1345,7 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1238,24 +1356,24 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1264,57 +1382,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1328,7 +1446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1336,7 +1454,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1345,7 +1463,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1354,7 +1472,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1363,7 +1481,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1372,7 +1490,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1381,7 +1499,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1390,7 +1508,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1399,7 +1517,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1408,7 +1526,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1417,7 +1535,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1426,7 +1544,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1435,7 +1553,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1444,7 +1562,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1453,7 +1571,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1462,7 +1580,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1471,7 +1589,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1480,7 +1598,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1508,11 +1626,11 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1524,24 +1642,24 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1550,73 +1668,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="32">
         <v>45872</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1630,7 +1748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="90">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1644,7 +1762,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1659,7 +1777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1674,7 +1792,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="120">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1689,7 +1807,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="90">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1704,7 +1822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1713,7 +1831,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1722,7 +1840,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1731,7 +1849,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1740,7 +1858,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1749,7 +1867,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1758,7 +1876,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1767,7 +1885,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1776,7 +1894,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1785,7 +1903,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1794,7 +1912,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1803,7 +1921,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1812,7 +1930,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1821,7 +1939,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1830,7 +1948,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1839,7 +1957,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1848,7 +1966,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1878,16 +1996,16 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
@@ -1895,24 +2013,24 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1921,47 +2039,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="32">
+        <v>45872</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1978,86 +2114,150 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="195">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="105">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="120">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="90">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="60">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="180">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2067,7 +2267,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2077,7 +2277,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2087,7 +2287,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2097,7 +2297,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2107,7 +2307,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2117,7 +2317,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2127,7 +2327,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2137,7 +2337,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2147,7 +2347,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2157,7 +2357,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2167,7 +2367,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2177,7 +2377,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2187,15 +2387,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6">
+      <c r="C32" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to add something in the report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geani\IdeaProjects\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ADB713-8377-4242-9696-833753D9952A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725B2EF-49AC-4E6D-A1C5-6D26B71F3AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19092" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -707,6 +707,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -751,9 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1085,19 +1085,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1117,10 +1117,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1131,10 +1131,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1146,15 +1146,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1361,19 +1361,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1393,10 +1393,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1407,10 +1407,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1422,15 +1422,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1647,19 +1647,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1683,10 +1683,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1701,10 +1701,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1720,19 +1720,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="33">
         <v>45872</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1996,8 +1996,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2018,19 +2018,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2054,10 +2054,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2072,10 +2072,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2091,10 +2091,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="33">
         <v>45872</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10">
@@ -2160,7 +2160,7 @@
       <c r="D12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="23" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -2388,12 +2388,14 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="18"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="18" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="6:6">
       <c r="F35" s="21"/>

</xml_diff>

<commit_message>
Updated Lab01 review report with architectural inspection
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geani\IdeaProjects\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Year3Sem2\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725B2EF-49AC-4E6D-A1C5-6D26B71F3AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685515FF-0C45-4FEF-AC5B-8CB671B4045F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19092" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -471,6 +471,124 @@
   </si>
   <si>
     <t>stage.setOnCloseRequest(Event::consume);</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>The Main class has too many responsabilities ( application startup, UI setup, payment reporting ) 
+	- Create an ApplicationContext class to handle initializations.
+OrdersGUIController mixes UI Control Logic with Business Calculations.
+	- Extract Business Logic from Controllers into Service Classes</t>
+  </si>
+  <si>
+    <t>PaymentAlert is in the service package but handles UI concerns.
+	- Reorganize packages to reflect logical layers and move PaymentAlert to a ui.dialog 	package.
+PizzaService integrates directly with Repositories without interfaces.
+	- Introduce interfaces for repositories to reduce coupling.</t>
+  </si>
+  <si>
+    <t>Main.java
+OrdersGUIController.java</t>
+  </si>
+  <si>
+    <t>PaymentAlert.java
+PizzaService.java</t>
+  </si>
+  <si>
+    <t>The Requirements about the conditions for closing the kitchen and restaurant are missing.
+      - Add verification logic for closing conditions in the architecture diagram.</t>
+  </si>
+  <si>
+    <t>Main.java
+RequirementsPizzaShop_v1.0.pdf</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java
+KitchenGUIController.java</t>
+  </si>
+  <si>
+    <t>OrdersGUIController calculates payment totals instead of delegating to a service.
+	- Add an OrderService class to handle business logic.
+KitchenGUIController manages a thread for UI updates.
+	- Add a ThreadManager to handle UI update operations.</t>
+  </si>
+  <si>
+    <t>KitchenGUI.java
+OrdersGUI.java</t>
+  </si>
+  <si>
+    <t>Many methods catch exceptions and just print stack traces (e.g., in KitchenGUI, OrdersGUI).
+	- Add an ErrorHandler class to the architecture.
+No validation for critical operations like payments.
+	- Include validation components in the diagram.</t>
+  </si>
+  <si>
+    <t>No clear use of Observer pattern for kitchen-server communication.
+	- Implement Observer pattern for kitchen notifications.
+Repository pattern exists but without interfaces.
+	- Add interfaces for repositories in the architecture.</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java</t>
+  </si>
+  <si>
+    <t>KitchenGUI.java
+PaymentAlert.java</t>
+  </si>
+  <si>
+    <t>KitchenGUI.KitchenGUI() method duplicates class name. 
+	-  Rename method to displayKitchenWindow().
+PaymentAlert handles both alerts and payment processing.
+	- Split PaymentAlert into PaymentDialogService and PaymentProcessor.</t>
+  </si>
+  <si>
+    <t>PizzaService.java
+Main.java</t>
+  </si>
+  <si>
+    <t>PizzaService handles both menu data and payment processing, which are distinct concerns. 
+	- Split PizzaService into MenuService and PaymentService.
+Main class includes payment reporting.
+	- Add a ReportingService</t>
+  </si>
+  <si>
+    <t>In the class diagram, many relationships lack names or multiplicity indicators.
+	- Add proper relationship names and multiplicity indicators to all associations in the updated class diagram.</t>
+  </si>
+  <si>
+    <t>Class diagram</t>
+  </si>
+  <si>
+    <t>There's no Order entity to represent customer orders in the architecture, which is a core business concept.
+	- Add an Order class with relationships to MenuItems, Table, and Payment classes in the updated diagram.</t>
   </si>
 </sst>
 </file>
@@ -675,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -710,6 +828,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -731,13 +852,13 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1068,36 +1189,36 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1117,10 +1238,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1131,10 +1252,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1146,15 +1267,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1341,39 +1462,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1386,51 +1507,67 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="32">
+        <v>45903</v>
+      </c>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1446,94 +1583,154 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="144">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="C10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="129.6">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="57.6">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="C12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="129.6">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="C13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="100.8">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="115.2">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="C15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="115.2">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="100.8">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="72">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="86.4">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="3">
@@ -1627,39 +1824,39 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E7"/>
+      <selection activeCell="H2" sqref="H2:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1683,10 +1880,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1701,10 +1898,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="37"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1720,19 +1917,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>45872</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1748,7 +1945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90">
+    <row r="10" spans="1:10" ht="86.4">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1762,7 +1959,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="43.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1777,7 +1974,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45">
+    <row r="12" spans="1:10" ht="43.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1792,7 +1989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="120">
+    <row r="13" spans="1:10" ht="100.8">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1807,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="90">
+    <row r="14" spans="1:10" ht="86.4">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1996,41 +2193,41 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2054,10 +2251,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="35"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2072,10 +2269,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2091,10 +2288,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <v>45872</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10">
@@ -2114,7 +2311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="195">
+    <row r="10" spans="1:10" ht="172.8">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2131,7 +2328,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="105">
+    <row r="11" spans="1:10" ht="100.8">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2167,7 +2364,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45">
+    <row r="13" spans="1:10" ht="28.8">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2185,7 +2382,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="120">
+    <row r="14" spans="1:10" ht="100.8">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2203,7 +2400,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="90">
+    <row r="15" spans="1:10" ht="57.6">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2221,7 +2418,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="60">
+    <row r="16" spans="1:10" ht="57.6">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2239,7 +2436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="180">
+    <row r="17" spans="2:6" ht="172.8">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2388,11 +2585,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="18" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Updated Lab01 review report with requirements inspection
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Year3Sem2\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40771\IdeaProjects\VVSS\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685515FF-0C45-4FEF-AC5B-8CB671B4045F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160B07B6-805F-4CAA-BB52-B8B81F538CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -589,6 +587,39 @@
   <si>
     <t>There's no Order entity to represent customer orders in the architecture, which is a core business concept.
 	- Add an Order class with relationships to MenuItems, Table, and Payment classes in the updated diagram.</t>
+  </si>
+  <si>
+    <t>10/3/2025</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>paragraful 2</t>
+  </si>
+  <si>
+    <t>paragraful 5</t>
+  </si>
+  <si>
+    <t>nu sunt retinute inainte datele necesate pentru efectuarea acestui pas</t>
+  </si>
+  <si>
+    <t>paragraful 7-8</t>
+  </si>
+  <si>
+    <t>conditia inchideri bucatariei este aceeasi ca si a restaurantului cu toate ca bucataria se poate inchide mai devreme</t>
+  </si>
+  <si>
+    <t>definera incompleta a unei comenzi: lipsa unui pret final sau a modului de plata</t>
+  </si>
+  <si>
+    <t>Lipsa unui  mod de a memora comenzile</t>
   </si>
 </sst>
 </file>
@@ -793,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -831,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -841,6 +872,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1185,8 +1219,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1231,8 +1265,12 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
@@ -1245,36 +1283,48 @@
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>114</v>
+      </c>
       <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10">
@@ -1291,40 +1341,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="28.8">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="C11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="C12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="3">
@@ -1462,7 +1536,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -1518,10 +1592,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1536,10 +1610,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1555,19 +1629,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="33">
         <v>45903</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1824,7 +1898,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J5"/>
+      <selection activeCell="I3" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1880,10 +1954,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1898,10 +1972,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1917,19 +1991,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="33">
         <v>45872</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2193,7 +2267,7 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -2251,10 +2325,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2269,10 +2343,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2288,10 +2362,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="33">
         <v>45872</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10">
@@ -2585,11 +2659,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="18" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Diagram + added checklist questions into the report
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40771\IdeaProjects\VVSS\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Year3Sem2\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160B07B6-805F-4CAA-BB52-B8B81F538CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B524672E-7555-4B21-939A-02CB8A707A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="117">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -471,36 +471,6 @@
     <t>stage.setOnCloseRequest(Event::consume);</t>
   </si>
   <si>
-    <t>A01</t>
-  </si>
-  <si>
-    <t>A02</t>
-  </si>
-  <si>
-    <t>A03</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
-    <t>A05</t>
-  </si>
-  <si>
-    <t>A06</t>
-  </si>
-  <si>
-    <t>A07</t>
-  </si>
-  <si>
-    <t>A08</t>
-  </si>
-  <si>
-    <t>A09</t>
-  </si>
-  <si>
-    <t>A010</t>
-  </si>
-  <si>
     <t>The Main class has too many responsabilities ( application startup, UI setup, payment reporting ) 
 	- Create an ApplicationContext class to handle initializations.
 OrdersGUIController mixes UI Control Logic with Business Calculations.
@@ -521,41 +491,12 @@
 PizzaService.java</t>
   </si>
   <si>
-    <t>The Requirements about the conditions for closing the kitchen and restaurant are missing.
-      - Add verification logic for closing conditions in the architecture diagram.</t>
-  </si>
-  <si>
     <t>Main.java
 RequirementsPizzaShop_v1.0.pdf</t>
   </si>
   <si>
-    <t>OrdersGUIController.java
-KitchenGUIController.java</t>
-  </si>
-  <si>
-    <t>OrdersGUIController calculates payment totals instead of delegating to a service.
-	- Add an OrderService class to handle business logic.
-KitchenGUIController manages a thread for UI updates.
-	- Add a ThreadManager to handle UI update operations.</t>
-  </si>
-  <si>
     <t>KitchenGUI.java
 OrdersGUI.java</t>
-  </si>
-  <si>
-    <t>Many methods catch exceptions and just print stack traces (e.g., in KitchenGUI, OrdersGUI).
-	- Add an ErrorHandler class to the architecture.
-No validation for critical operations like payments.
-	- Include validation components in the diagram.</t>
-  </si>
-  <si>
-    <t>No clear use of Observer pattern for kitchen-server communication.
-	- Implement Observer pattern for kitchen notifications.
-Repository pattern exists but without interfaces.
-	- Add interfaces for repositories in the architecture.</t>
-  </si>
-  <si>
-    <t>KitchenGUIController.java</t>
   </si>
   <si>
     <t>KitchenGUI.java
@@ -578,10 +519,6 @@
 	- Add a ReportingService</t>
   </si>
   <si>
-    <t>In the class diagram, many relationships lack names or multiplicity indicators.
-	- Add proper relationship names and multiplicity indicators to all associations in the updated class diagram.</t>
-  </si>
-  <si>
     <t>Class diagram</t>
   </si>
   <si>
@@ -620,6 +557,37 @@
   </si>
   <si>
     <t>Lipsa unui  mod de a memora comenzile</t>
+  </si>
+  <si>
+    <t>A01 : Is the overall organization of the program clear, including good architectural overview?</t>
+  </si>
+  <si>
+    <t>A02 : Is the subsystem and package partitioning and layering logically consistent?</t>
+  </si>
+  <si>
+    <t>A03 : Does the architecture account for all of the requirements?</t>
+  </si>
+  <si>
+    <t>The Requirements about the conditions for closing the kitchen and restaurant are missing.
+      - Add verification logic for closing conditions.</t>
+  </si>
+  <si>
+    <t>A05 : Is there a coherent error handling strategy provided?</t>
+  </si>
+  <si>
+    <t>A07 : Is the name and description of each class clearly reflecting the played role ?</t>
+  </si>
+  <si>
+    <t>A08 : Is the description of each class accurately capturing the responsibilities of the class?</t>
+  </si>
+  <si>
+    <t>A010 : Are the key entity classes and their relationships consistent with the business model (if it exists), domain model (if it exists), requirements?</t>
+  </si>
+  <si>
+    <t>Many methods catch exceptions and just print stack traces (e.g., in KitchenGUI, OrdersGUI).
+	- Add an ErrorHandler class to the architecture.
+No validation for critical operations like payments.
+	- Include validation components.</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1187,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1323,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -1346,13 +1314,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1361,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8">
@@ -1376,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2">
@@ -1391,13 +1359,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1536,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E16" sqref="C10:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1661,14 +1629,14 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="129.6">
@@ -1676,14 +1644,14 @@
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.6">
@@ -1691,120 +1659,102 @@
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>87</v>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="129.6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="100.8">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>88</v>
+      <c r="C13" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="100.8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="115.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>89</v>
+      <c r="C14" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="115.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="100.8">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>106</v>
+      <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="115.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="129.6">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>91</v>
+      <c r="C16" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="100.8">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="72">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="86.4">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="3">
@@ -1897,7 +1847,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I3" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
@@ -2267,7 +2217,7 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added checked item descriptions in code review tab
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Year3Sem2\VVSS\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geani\IdeaProjects\VVSS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B524672E-7555-4B21-939A-02CB8A707A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E2644-4AB7-4F4A-B093-1E1A884EC9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Ciulavu Dan Flaviu</t>
-  </si>
-  <si>
-    <t>C09</t>
   </si>
   <si>
     <t>OrdersGUI.java/line 22</t>
@@ -230,15 +227,9 @@
     </r>
   </si>
   <si>
-    <t>C06</t>
-  </si>
-  <si>
     <t>Folosim rezultatul unui Optional fara sa verificam daca exista unul. Cazul de exceptie in care nu avem niciun rezultat trebuie tratat.</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>PizzaService.java/line 32</t>
   </si>
   <si>
@@ -246,9 +237,6 @@
   </si>
   <si>
     <t>OrdersGUIController.java/line 150; PaymentAlert/line 46, 49</t>
-  </si>
-  <si>
-    <t>C08</t>
   </si>
   <si>
     <t>MenuRepository.java/line 48</t>
@@ -588,6 +576,18 @@
 	- Add an ErrorHandler class to the architecture.
 No validation for critical operations like payments.
 	- Include validation components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C08: Error message processing errors exist. </t>
+  </si>
+  <si>
+    <t>C11: Errors are made in writing out variable names.</t>
+  </si>
+  <si>
+    <t>C06: There are errors in preparing or processing input data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C09: There is confusion in the use of parameters. </t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E7" s="25"/>
     </row>
@@ -1314,13 +1314,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8">
@@ -1344,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2">
@@ -1359,13 +1359,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1504,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E16" sqref="C10:E16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1630,13 +1630,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="129.6">
@@ -1645,13 +1645,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="57.6">
@@ -1660,13 +1660,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="100.8">
@@ -1675,13 +1675,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="115.2">
@@ -1690,13 +1690,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="100.8">
@@ -1705,13 +1705,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="129.6">
@@ -1720,13 +1720,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -1847,15 +1847,15 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="35.44140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
@@ -1974,13 +1974,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2">
@@ -1989,13 +1989,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.2">
@@ -2004,13 +2004,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="100.8">
@@ -2019,13 +2019,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="86.4">
@@ -2034,13 +2034,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2276,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
@@ -2340,16 +2340,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="100.8">
@@ -2358,16 +2358,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2376,16 +2376,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8">
@@ -2394,16 +2394,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="100.8">
@@ -2412,16 +2412,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="57.6">
@@ -2430,16 +2430,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="57.6">
@@ -2448,16 +2448,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="172.8">
@@ -2466,16 +2466,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -2615,7 +2615,7 @@
       <c r="D32" s="40"/>
       <c r="E32" s="40"/>
       <c r="F32" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="6:6">

</xml_diff>